<commit_message>
Changes to PDFs and Docs
</commit_message>
<xml_diff>
--- a/Data/SMcalculation.xlsx
+++ b/Data/SMcalculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="27320" windowHeight="13160" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="27320" windowHeight="13160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Fine Sand" sheetId="5" r:id="rId1"/>
@@ -565,6 +565,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,9 +595,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -593,18 +605,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -995,11 +995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1130698096"/>
-        <c:axId val="1130701216"/>
+        <c:axId val="3121440"/>
+        <c:axId val="3122304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1130698096"/>
+        <c:axId val="3121440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,12 +1141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130701216"/>
+        <c:crossAx val="3122304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1130701216"/>
+        <c:axId val="3122304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130698096"/>
+        <c:crossAx val="3121440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2523,11 +2523,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1129819856"/>
-        <c:axId val="1129824400"/>
+        <c:axId val="1958688"/>
+        <c:axId val="1963232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1129819856"/>
+        <c:axId val="1958688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2540,7 +2540,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2572,7 +2572,31 @@
                     <a:ea typeface="Times" charset="0"/>
                     <a:cs typeface="Times" charset="0"/>
                   </a:rPr>
-                  <a:t> head (cm)</a:t>
+                  <a:t> head </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>𝜓𝑠</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times" charset="0"/>
+                    <a:ea typeface="Times" charset="0"/>
+                    <a:cs typeface="Times" charset="0"/>
+                  </a:rPr>
+                  <a:t> (cm)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1100" b="1">
                   <a:solidFill>
@@ -2599,7 +2623,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2646,12 +2670,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129824400"/>
+        <c:crossAx val="1963232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1129824400"/>
+        <c:axId val="1963232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2696,7 +2720,7 @@
                     <a:ea typeface="Times" charset="0"/>
                     <a:cs typeface="Times" charset="0"/>
                   </a:rPr>
-                  <a:t> Water Content (cm3/cm3)</a:t>
+                  <a:t> Water Content ϴ (cm3/cm3)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1100" b="1">
                   <a:solidFill>
@@ -2770,7 +2794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129819856"/>
+        <c:crossAx val="1958688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2825,16 +2849,9 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3260,11 +3277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1129462464"/>
-        <c:axId val="1129465856"/>
+        <c:axId val="1759968"/>
+        <c:axId val="1764000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1129462464"/>
+        <c:axId val="1759968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3398,12 +3415,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129465856"/>
+        <c:crossAx val="1764000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1129465856"/>
+        <c:axId val="1764000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3545,7 +3562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129462464"/>
+        <c:crossAx val="1759968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3930,11 +3947,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1064706944"/>
-        <c:axId val="1129406048"/>
+        <c:axId val="1803072"/>
+        <c:axId val="1807104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1064706944"/>
+        <c:axId val="1803072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4076,12 +4093,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129406048"/>
+        <c:crossAx val="1807104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1129406048"/>
+        <c:axId val="1807104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,7 +4204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1064706944"/>
+        <c:crossAx val="1803072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4290,7 +4307,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4639,11 +4655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1064334480"/>
-        <c:axId val="1064343104"/>
+        <c:axId val="1830896"/>
+        <c:axId val="1834928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1064334480"/>
+        <c:axId val="1830896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4777,12 +4793,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1064343104"/>
+        <c:crossAx val="1834928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1064343104"/>
+        <c:axId val="1834928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4924,7 +4940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1064334480"/>
+        <c:crossAx val="1830896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5309,11 +5325,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1109826448"/>
-        <c:axId val="1110392112"/>
+        <c:axId val="1850128"/>
+        <c:axId val="1854160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1109826448"/>
+        <c:axId val="1850128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5455,12 +5471,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1110392112"/>
+        <c:crossAx val="1854160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1110392112"/>
+        <c:axId val="1854160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5566,7 +5582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1109826448"/>
+        <c:crossAx val="1850128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6017,11 +6033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1130903888"/>
-        <c:axId val="1130907008"/>
+        <c:axId val="1879264"/>
+        <c:axId val="1883296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1130903888"/>
+        <c:axId val="1879264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -6155,12 +6171,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130907008"/>
+        <c:crossAx val="1883296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1130907008"/>
+        <c:axId val="1883296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6302,7 +6318,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130903888"/>
+        <c:crossAx val="1879264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6687,11 +6703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1039959696"/>
-        <c:axId val="1064365056"/>
+        <c:axId val="1904032"/>
+        <c:axId val="1908064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1039959696"/>
+        <c:axId val="1904032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6833,12 +6849,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1064365056"/>
+        <c:crossAx val="1908064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1064365056"/>
+        <c:axId val="1908064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6944,7 +6960,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1039959696"/>
+        <c:crossAx val="1904032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7395,11 +7411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1110420560"/>
-        <c:axId val="1110423952"/>
+        <c:axId val="3170144"/>
+        <c:axId val="3174176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1110420560"/>
+        <c:axId val="3170144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -7533,12 +7549,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1110423952"/>
+        <c:crossAx val="3174176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1110423952"/>
+        <c:axId val="3174176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7680,7 +7696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1110420560"/>
+        <c:crossAx val="3170144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8951,11 +8967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1064616768"/>
-        <c:axId val="1129487648"/>
+        <c:axId val="3223696"/>
+        <c:axId val="3228240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1064616768"/>
+        <c:axId val="3223696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -9092,12 +9108,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1129487648"/>
+        <c:crossAx val="3228240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1129487648"/>
+        <c:axId val="3228240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9214,7 +9230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1064616768"/>
+        <c:crossAx val="3223696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21484,8 +21500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V134"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54:G116"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21502,10 +21518,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="47"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="24"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -21519,31 +21535,31 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="2:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="22"/>
       <c r="E2" s="12"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
     </row>
     <row r="3" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -21553,26 +21569,26 @@
         <v>41</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
     </row>
     <row r="4" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -21584,22 +21600,22 @@
       <c r="D4" s="23"/>
       <c r="E4" s="12"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
     </row>
     <row r="5" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -21611,24 +21627,24 @@
       <c r="D5" s="23"/>
       <c r="E5" s="12"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53" t="s">
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
     </row>
     <row r="6" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
@@ -21636,26 +21652,26 @@
       <c r="D6" s="23"/>
       <c r="E6" s="12"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
     </row>
     <row r="7" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
@@ -21668,23 +21684,23 @@
       <c r="D7" s="2"/>
       <c r="E7" s="12"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="58" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="2:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
@@ -21697,16 +21713,16 @@
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="60" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -23053,26 +23069,26 @@
       <c r="D2" s="22"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
     </row>
     <row r="3" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -23082,26 +23098,26 @@
         <v>12.41</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
     </row>
     <row r="4" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -23113,22 +23129,22 @@
       <c r="D4" s="23"/>
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
     </row>
     <row r="5" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -23140,24 +23156,24 @@
       <c r="D5" s="23"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53" t="s">
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
     </row>
     <row r="6" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
@@ -23165,26 +23181,26 @@
       <c r="D6" s="23"/>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
     </row>
     <row r="7" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
@@ -23197,23 +23213,23 @@
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="58" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="2:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
@@ -23226,16 +23242,16 @@
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="60" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -24518,26 +24534,26 @@
       <c r="D2" s="22"/>
       <c r="E2" s="12"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
     </row>
     <row r="3" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -24547,26 +24563,26 @@
         <v>78.599999999999994</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
     </row>
     <row r="4" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -24578,22 +24594,22 @@
       <c r="D4" s="23"/>
       <c r="E4" s="12"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
     </row>
     <row r="5" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -24605,24 +24621,24 @@
       <c r="D5" s="23"/>
       <c r="E5" s="12"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53" t="s">
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
     </row>
     <row r="6" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
@@ -24630,26 +24646,26 @@
       <c r="D6" s="23"/>
       <c r="E6" s="12"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
     </row>
     <row r="7" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
@@ -24662,23 +24678,23 @@
       <c r="D7" s="2"/>
       <c r="E7" s="12"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="58" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="2:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
@@ -24691,16 +24707,16 @@
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="60" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -25983,26 +25999,26 @@
       <c r="D2" s="22"/>
       <c r="E2" s="12"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
     </row>
     <row r="3" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -26012,26 +26028,26 @@
         <v>35.6</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
     </row>
     <row r="4" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -26043,22 +26059,22 @@
       <c r="D4" s="23"/>
       <c r="E4" s="12"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
     </row>
     <row r="5" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -26070,24 +26086,24 @@
       <c r="D5" s="23"/>
       <c r="E5" s="12"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53" t="s">
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
     </row>
     <row r="6" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
@@ -26095,26 +26111,26 @@
       <c r="D6" s="23"/>
       <c r="E6" s="12"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
     </row>
     <row r="7" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
@@ -26127,23 +26143,23 @@
       <c r="D7" s="2"/>
       <c r="E7" s="12"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="58" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="2:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
@@ -26156,16 +26172,16 @@
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="60" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -28179,8 +28195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28963,7 +28979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>

</xml_diff>